<commit_message>
Updated results/model outputs for GAMMs
</commit_message>
<xml_diff>
--- a/results/Activity Scope/gamm_fs_param_ind.xlsx
+++ b/results/Activity Scope/gamm_fs_param_ind.xlsx
@@ -395,7 +395,7 @@
         <v>0.445052644423581</v>
       </c>
       <c r="D2" t="n">
-        <v>87.4253196385777</v>
+        <v>87.4253196385778</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -415,7 +415,7 @@
         <v>-10.5582452918197</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000000000000000000000000736771873303689</v>
+        <v>0.000000000000000000000000736771873303593</v>
       </c>
     </row>
     <row r="4">
@@ -423,16 +423,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>-4.08866220401575</v>
+        <v>-4.08866220401576</v>
       </c>
       <c r="C4" t="n">
         <v>0.516317698783061</v>
       </c>
       <c r="D4" t="n">
-        <v>-7.91888833881262</v>
+        <v>-7.91888833881263</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00000000000000596230307326945</v>
+        <v>0.00000000000000596230307326902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>